<commit_message>
November date fix and prliminary graph for parks people
</commit_message>
<xml_diff>
--- a/GW_seaweed_seasonality_transect_data1.xlsx
+++ b/GW_seaweed_seasonality_transect_data1.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{38EC0476-1FF6-4D41-9D9E-0D99C2282F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5902DE83-3E1C-4EBA-A862-CA6C975BE036}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{38EC0476-1FF6-4D41-9D9E-0D99C2282F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E49D589-CA14-46C2-9606-ACFA27C12C6F}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">in!$A$1:$N$117</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -566,9 +569,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -927,7 +931,8 @@
   <dimension ref="A1:N117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,51 +941,52 @@
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2218,7 +2224,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>44506</v>
+        <v>44505</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2235,7 +2241,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>44507</v>
+        <v>44505</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2255,7 +2261,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>44508</v>
+        <v>44505</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2269,7 +2275,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>44509</v>
+        <v>44505</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2286,7 +2292,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>44510</v>
+        <v>44505</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2306,7 +2312,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>44511</v>
+        <v>44505</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2320,7 +2326,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>44512</v>
+        <v>44505</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2340,7 +2346,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>44513</v>
+        <v>44505</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2354,7 +2360,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>44514</v>
+        <v>44505</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2377,7 +2383,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>44515</v>
+        <v>44505</v>
       </c>
       <c r="B78">
         <v>2</v>
@@ -2397,7 +2403,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>44516</v>
+        <v>44505</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -2414,7 +2420,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>44517</v>
+        <v>44505</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -2434,7 +2440,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>44518</v>
+        <v>44505</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -2448,7 +2454,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>44519</v>
+        <v>44505</v>
       </c>
       <c r="B82">
         <v>2</v>
@@ -2465,7 +2471,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>44520</v>
+        <v>44505</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -2488,7 +2494,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>44521</v>
+        <v>44505</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -2505,7 +2511,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>44522</v>
+        <v>44505</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -2531,7 +2537,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>44523</v>
+        <v>44505</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -2551,7 +2557,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>44524</v>
+        <v>44505</v>
       </c>
       <c r="B87">
         <v>3</v>
@@ -2565,7 +2571,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>44525</v>
+        <v>44505</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -2579,7 +2585,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>44526</v>
+        <v>44505</v>
       </c>
       <c r="B89">
         <v>3</v>
@@ -2599,7 +2605,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>44527</v>
+        <v>44505</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -2613,7 +2619,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>44528</v>
+        <v>44505</v>
       </c>
       <c r="B91">
         <v>3</v>
@@ -2627,7 +2633,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>44529</v>
+        <v>44505</v>
       </c>
       <c r="B92">
         <v>3</v>
@@ -2644,7 +2650,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>44530</v>
+        <v>44505</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -2661,7 +2667,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>44531</v>
+        <v>44505</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -2678,7 +2684,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>44532</v>
+        <v>44505</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -2695,7 +2701,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>44533</v>
+        <v>44505</v>
       </c>
       <c r="B96">
         <v>4</v>
@@ -2715,7 +2721,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>44534</v>
+        <v>44505</v>
       </c>
       <c r="B97">
         <v>4</v>
@@ -2735,7 +2741,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>44535</v>
+        <v>44505</v>
       </c>
       <c r="B98">
         <v>4</v>
@@ -2755,7 +2761,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>44536</v>
+        <v>44505</v>
       </c>
       <c r="B99">
         <v>4</v>
@@ -2775,7 +2781,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>44537</v>
+        <v>44505</v>
       </c>
       <c r="B100">
         <v>4</v>
@@ -2789,7 +2795,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
-        <v>44538</v>
+        <v>44505</v>
       </c>
       <c r="B101">
         <v>4</v>
@@ -2803,7 +2809,7 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>44539</v>
+        <v>44505</v>
       </c>
       <c r="B102">
         <v>4</v>
@@ -2823,7 +2829,7 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>44540</v>
+        <v>44505</v>
       </c>
       <c r="B103">
         <v>4</v>
@@ -2849,7 +2855,7 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
-        <v>44541</v>
+        <v>44505</v>
       </c>
       <c r="B104">
         <v>4</v>
@@ -2869,7 +2875,7 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
-        <v>44542</v>
+        <v>44505</v>
       </c>
       <c r="B105">
         <v>4</v>
@@ -2895,7 +2901,7 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
-        <v>44543</v>
+        <v>44505</v>
       </c>
       <c r="B106">
         <v>4</v>
@@ -2915,7 +2921,7 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
-        <v>44544</v>
+        <v>44505</v>
       </c>
       <c r="B107">
         <v>4</v>
@@ -2950,7 +2956,7 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
-        <v>44545</v>
+        <v>44505</v>
       </c>
       <c r="B108">
         <v>5</v>
@@ -2970,7 +2976,7 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
-        <v>44546</v>
+        <v>44505</v>
       </c>
       <c r="B109">
         <v>5</v>
@@ -2993,7 +2999,7 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
-        <v>44547</v>
+        <v>44505</v>
       </c>
       <c r="B110">
         <v>5</v>
@@ -3013,7 +3019,7 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
-        <v>44548</v>
+        <v>44505</v>
       </c>
       <c r="B111">
         <v>5</v>
@@ -3033,7 +3039,7 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
-        <v>44549</v>
+        <v>44505</v>
       </c>
       <c r="B112">
         <v>5</v>
@@ -3053,7 +3059,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
-        <v>44550</v>
+        <v>44505</v>
       </c>
       <c r="B113">
         <v>5</v>
@@ -3070,7 +3076,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
-        <v>44551</v>
+        <v>44505</v>
       </c>
       <c r="B114">
         <v>5</v>
@@ -3090,7 +3096,7 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
-        <v>44552</v>
+        <v>44505</v>
       </c>
       <c r="B115">
         <v>5</v>
@@ -3107,7 +3113,7 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
-        <v>44553</v>
+        <v>44505</v>
       </c>
       <c r="B116">
         <v>5</v>
@@ -3136,7 +3142,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
-        <v>44554</v>
+        <v>44505</v>
       </c>
       <c r="B117">
         <v>5</v>
@@ -3164,6 +3170,8 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N117" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>